<commit_message>
tout test traitement fonctionnel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.thevenet\PhpstormProjects\untitled5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42480DEF-461B-4265-A9E9-CE4A1E7F8DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C20FAFB-36FB-47DF-B59B-2EEF0A78E03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{5B1F9352-606B-4A97-B055-F467C123F5D1}"/>
+    <workbookView xWindow="2595" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{5B1F9352-606B-4A97-B055-F467C123F5D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>prix</t>
   </si>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14EC2A6-FB83-480A-A4C3-15C8142D1600}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -526,6 +526,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>